<commit_message>
Fix: ajustes contribuir, lancamentos importacao, layout mobile
</commit_message>
<xml_diff>
--- a/public/modelo_importacao_cartao-credito.xlsx
+++ b/public/modelo_importacao_cartao-credito.xlsx
@@ -24,9 +24,6 @@
     <t>banco</t>
   </si>
   <si>
-    <t>nome_cartao</t>
-  </si>
-  <si>
     <t>fatura_mes</t>
   </si>
   <si>
@@ -81,13 +78,16 @@
     <t>Alimentação</t>
   </si>
   <si>
-    <t>Supermercados 123</t>
-  </si>
-  <si>
     <t>sub_categoria</t>
   </si>
   <si>
     <t>Supermercados</t>
+  </si>
+  <si>
+    <t>nome_cartao_credito</t>
+  </si>
+  <si>
+    <t>Supermercados ABC</t>
   </si>
 </sst>
 </file>
@@ -470,72 +470,72 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2">
+        <v>400</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="2">
-        <v>600</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="K2" s="2">
         <v>1</v>
@@ -544,7 +544,7 @@
         <v>4</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>